<commit_message>
Horizontal and vertical lines added , Look designed in tabular format .
</commit_message>
<xml_diff>
--- a/Invoice.xlsx
+++ b/Invoice.xlsx
@@ -14,36 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cust_name</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Wagvilasinee Kulkarni</t>
   </si>
   <si>
-    <t>Devashree Deolankar</t>
-  </si>
-  <si>
-    <t>Shreyas Joshi</t>
-  </si>
-  <si>
-    <t>Mukta Chandrachud</t>
-  </si>
-  <si>
-    <t>Nitin Tare</t>
-  </si>
-  <si>
     <t>Sr.No</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Previous_pending</t>
+  </si>
+  <si>
+    <t>CM_total</t>
+  </si>
+  <si>
+    <t>C_rate</t>
+  </si>
+  <si>
+    <t>B_rate</t>
+  </si>
+  <si>
+    <t>BM_total</t>
   </si>
 </sst>
 </file>
@@ -385,126 +391,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>30</v>
       </c>
       <c r="D2">
-        <v>55.5</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <f>D2*C2</f>
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+        <v>1500</v>
+      </c>
+      <c r="F2">
         <v>60</v>
       </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <f>D3*C3</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
+      <c r="G2">
         <v>75</v>
       </c>
-      <c r="E4">
-        <f>D4*C4</f>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>80</v>
-      </c>
-      <c r="E5">
-        <f>D5*C5</f>
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>28</v>
-      </c>
-      <c r="D6">
-        <v>60</v>
-      </c>
-      <c r="E6">
-        <f>D6*C6</f>
-        <v>1680</v>
+      <c r="H2">
+        <f>G2*F2</f>
+        <v>4500</v>
+      </c>
+      <c r="I2">
+        <v>250</v>
+      </c>
+      <c r="J2">
+        <v>500</v>
+      </c>
+      <c r="K2">
+        <f>E2+H2+I2+J2</f>
+        <v>6750</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added QR code image and code
</commit_message>
<xml_diff>
--- a/Invoice.xlsx
+++ b/Invoice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Cust_name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>BM_total</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
@@ -85,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,9 +411,10 @@
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -440,8 +448,11 @@
       <c r="K1" t="s">
         <v>1</v>
       </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,6 +488,9 @@
       <c r="K2">
         <f>E2+H2+I2+J2</f>
         <v>6750</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>